<commit_message>
ignore string upper/lower case
</commit_message>
<xml_diff>
--- a/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
+++ b/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -261,10 +261,10 @@
     <t>TS_7</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>eat</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,13 +736,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -761,9 +761,6 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -784,9 +781,6 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -807,9 +801,6 @@
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -828,9 +819,6 @@
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -849,10 +837,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -870,9 +855,6 @@
         <v>12</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
cater case for browser type in test data
</commit_message>
<xml_diff>
--- a/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
+++ b/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="81">
   <si>
     <t>Description</t>
   </si>
@@ -264,10 +264,13 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>openbrowsers</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>openbrowser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
         <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,7 +689,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +745,7 @@
         <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -761,6 +764,9 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -781,6 +787,9 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -801,6 +810,9 @@
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -819,6 +831,9 @@
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -839,6 +854,9 @@
       <c r="F7" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -855,6 +873,9 @@
         <v>12</v>
       </c>
       <c r="F8" s="7"/>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -995,7 +1016,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1052,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cater case sensitivity for testcaseID for step counter
</commit_message>
<xml_diff>
--- a/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
+++ b/Hybrid Keyword Driven/src/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="82">
   <si>
     <t>Description</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
   <si>
     <t>PASS</t>
@@ -617,7 +620,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +656,7 @@
         <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +748,7 @@
         <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -765,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,12 +791,12 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -811,7 +814,7 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,7 +858,7 @@
         <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -874,7 +877,7 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1016,7 +1019,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>

</xml_diff>